<commit_message>
Now with Reasons Reflection and updated PDF report - V0.1
</commit_message>
<xml_diff>
--- a/src/data/Money Survey V1.0 - Data for App.xlsx
+++ b/src/data/Money Survey V1.0 - Data for App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\financial-wellbeing-app\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0E1BB1-A216-471F-A716-4BF9820FB4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E040B525-8CF2-46EF-A979-CB22CE41D868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2865" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="139">
   <si>
     <t>How good are you at money? Let's find out by answering some questions…</t>
   </si>
@@ -240,18 +240,9 @@
     <t>Do you keep up to date with the latest types of scams and how to spot them?</t>
   </si>
   <si>
-    <t>What’s Stopping you get better at money? Select Yes or Somewhat. Then rank your top 3 reasons.</t>
-  </si>
-  <si>
-    <t>Top 3</t>
-  </si>
-  <si>
     <t>I am not that motivated to do anything about it</t>
   </si>
   <si>
-    <t>Somewhat</t>
-  </si>
-  <si>
     <t>I am already good enough with money</t>
   </si>
   <si>
@@ -276,9 +267,6 @@
     <t>I cannot control or do not want to control my spending</t>
   </si>
   <si>
-    <t>I have limited or no financial literacy (budgeting, compounding, super, credit)</t>
-  </si>
-  <si>
     <t>I don’t wont to have to create or run a budget</t>
   </si>
   <si>
@@ -327,9 +315,6 @@
     <t>I cannot afford the cost of getting help</t>
   </si>
   <si>
-    <t xml:space="preserve">Other (Please Specify) : </t>
-  </si>
-  <si>
     <t>I have been burnt before</t>
   </si>
   <si>
@@ -469,13 +454,19 @@
   </si>
   <si>
     <t>re_J8BPpLQT_8eTYwn5ZstWPxgGxCYeLbA7a</t>
+  </si>
+  <si>
+    <t>Demotivators</t>
+  </si>
+  <si>
+    <t>I have limited or no financial literacy (e.g. budgeting, compounding, super, credit)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,28 +477,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos"/>
-      <family val="18"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -528,15 +497,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,18 +507,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -564,20 +520,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="dotted">
-        <color rgb="FF505050"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -585,25 +532,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -958,7 +893,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -984,13 +919,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1009,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1020,7 +955,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1031,7 +966,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -1042,7 +977,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -1053,7 +988,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -1064,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -1075,7 +1010,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
         <v>43</v>
@@ -1086,7 +1021,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
         <v>48</v>
@@ -1097,7 +1032,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
         <v>53</v>
@@ -1108,7 +1043,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C12" t="s">
         <v>56</v>
@@ -1119,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
         <v>60</v>
@@ -1137,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A68A07C-A95D-0B45-B4E1-0FBF27F98BB9}">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,39 +1091,39 @@
     <col min="12" max="12" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="K1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="L1" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1198,7 +1133,7 @@
       <c r="B2" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1213,13 +1148,13 @@
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
-      <c r="I2" s="11">
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
         <v>2.1</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
@@ -1230,8 +1165,8 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>111</v>
+      <c r="C3" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -1245,13 +1180,13 @@
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="5">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="11"/>
+      <c r="J3" s="5"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
@@ -1262,8 +1197,8 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>112</v>
+      <c r="C4" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -1277,13 +1212,13 @@
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="5">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="5"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
@@ -1294,8 +1229,8 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>113</v>
+      <c r="C5" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>3</v>
@@ -1309,13 +1244,13 @@
       <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="5">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
@@ -1326,8 +1261,8 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>114</v>
+      <c r="C6" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
@@ -1341,13 +1276,13 @@
       <c r="G6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="5">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="11"/>
+      <c r="J6" s="5"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
@@ -1358,8 +1293,8 @@
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>115</v>
+      <c r="C7" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
@@ -1373,13 +1308,13 @@
       <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="5">
         <v>0</v>
       </c>
       <c r="I7" s="2">
         <v>2.1</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -1390,7 +1325,7 @@
       <c r="B8" s="2">
         <v>2.1</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1405,13 +1340,13 @@
       <c r="G8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="11">
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
@@ -1422,8 +1357,8 @@
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>118</v>
+      <c r="C9" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -1437,13 +1372,13 @@
       <c r="G9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9" s="11" t="s">
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="11"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
@@ -1454,8 +1389,8 @@
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>119</v>
+      <c r="C10" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
@@ -1469,13 +1404,13 @@
       <c r="G10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10" s="11">
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J10" s="11"/>
+      <c r="J10" s="5"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
@@ -1486,7 +1421,7 @@
       <c r="B11" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1501,19 +1436,19 @@
       <c r="G11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="11">
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
         <v>3.1</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K11" s="11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="11">
+      <c r="J11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
         <v>3.1</v>
       </c>
     </row>
@@ -1524,7 +1459,7 @@
       <c r="B12" s="2">
         <v>3.1</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1539,10 +1474,10 @@
       <c r="G12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="11">
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -1553,8 +1488,8 @@
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>120</v>
+      <c r="C13" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>3</v>
@@ -1568,10 +1503,10 @@
       <c r="G13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="11">
-        <v>0</v>
-      </c>
-      <c r="I13" s="11" t="s">
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1582,8 +1517,8 @@
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>121</v>
+      <c r="C14" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>3</v>
@@ -1597,10 +1532,10 @@
       <c r="G14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="11">
-        <v>0</v>
-      </c>
-      <c r="I14" s="11">
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -1611,7 +1546,7 @@
       <c r="B15" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1626,16 +1561,16 @@
       <c r="G15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="5">
         <v>2</v>
       </c>
       <c r="I15" s="2">
         <v>4.2</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K15" s="11">
+      <c r="J15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="5">
         <v>0</v>
       </c>
       <c r="L15" s="2">
@@ -1649,7 +1584,7 @@
       <c r="B16" s="2">
         <v>4.2</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1664,16 +1599,16 @@
       <c r="G16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="5">
         <v>0</v>
       </c>
       <c r="I16" s="2">
         <v>4.3</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K16" s="11">
+      <c r="J16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="5">
         <v>0</v>
       </c>
       <c r="L16" s="2">
@@ -1687,7 +1622,7 @@
       <c r="B17" s="2">
         <v>4.3</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1702,14 +1637,14 @@
       <c r="G17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="11">
-        <v>0</v>
-      </c>
-      <c r="I17" s="11">
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1719,8 +1654,8 @@
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>125</v>
+      <c r="C18" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>3</v>
@@ -1734,14 +1669,14 @@
       <c r="G18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="11">
-        <v>0</v>
-      </c>
-      <c r="I18" s="11" t="s">
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1751,8 +1686,8 @@
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>126</v>
+      <c r="C19" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>3</v>
@@ -1766,14 +1701,14 @@
       <c r="G19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="11">
-        <v>0</v>
-      </c>
-      <c r="I19" s="11">
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1783,7 +1718,7 @@
       <c r="B20" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1798,16 +1733,16 @@
       <c r="G20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="5">
         <v>0</v>
       </c>
       <c r="I20" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J20" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K20" s="11">
+      <c r="J20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K20" s="5">
         <v>1</v>
       </c>
       <c r="L20" s="2">
@@ -1821,7 +1756,7 @@
       <c r="B21" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1836,14 +1771,14 @@
       <c r="G21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="11">
-        <v>2</v>
-      </c>
-      <c r="I21" s="11">
+      <c r="H21" s="5">
+        <v>2</v>
+      </c>
+      <c r="I21" s="5">
         <v>5.2</v>
       </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1853,8 +1788,8 @@
       <c r="B22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>127</v>
+      <c r="C22" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>3</v>
@@ -1868,19 +1803,19 @@
       <c r="G22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="5">
         <v>1</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K22" s="11">
-        <v>0</v>
-      </c>
-      <c r="L22" s="11" t="s">
+      <c r="J22" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1891,8 +1826,8 @@
       <c r="B23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>128</v>
+      <c r="C23" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>3</v>
@@ -1906,15 +1841,15 @@
       <c r="G23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="11">
-        <v>0</v>
-      </c>
-      <c r="I23" s="11">
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
         <v>5.2</v>
       </c>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -1923,7 +1858,7 @@
       <c r="B24" s="2">
         <v>5.2</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1938,15 +1873,15 @@
       <c r="G24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="11">
-        <v>2</v>
-      </c>
-      <c r="I24" s="11">
+      <c r="H24" s="5">
+        <v>2</v>
+      </c>
+      <c r="I24" s="5">
         <v>5.3</v>
       </c>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -1955,8 +1890,8 @@
       <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>129</v>
+      <c r="C25" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>3</v>
@@ -1970,19 +1905,19 @@
       <c r="G25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="5">
         <v>1</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="5">
         <v>5.3</v>
       </c>
-      <c r="J25" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K25" s="11">
-        <v>0</v>
-      </c>
-      <c r="L25" s="11" t="s">
+      <c r="J25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1993,7 +1928,7 @@
       <c r="B26" s="2">
         <v>5.3</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -2008,15 +1943,15 @@
       <c r="G26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="11">
-        <v>2</v>
-      </c>
-      <c r="I26" s="11">
+      <c r="H26" s="5">
+        <v>2</v>
+      </c>
+      <c r="I26" s="5">
         <v>5.4</v>
       </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -2025,8 +1960,8 @@
       <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>130</v>
+      <c r="C27" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>3</v>
@@ -2040,15 +1975,15 @@
       <c r="G27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="11">
-        <v>0</v>
-      </c>
-      <c r="I27" s="11">
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
         <v>5.4</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -2057,7 +1992,7 @@
       <c r="B28" s="2">
         <v>5.4</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -2072,15 +2007,15 @@
       <c r="G28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="11">
-        <v>2</v>
-      </c>
-      <c r="I28" s="11">
+      <c r="H28" s="5">
+        <v>2</v>
+      </c>
+      <c r="I28" s="5">
         <v>6.1</v>
       </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -2089,7 +2024,7 @@
       <c r="B29" s="2">
         <v>6.1</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -2104,15 +2039,15 @@
       <c r="G29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="11">
-        <v>0</v>
-      </c>
-      <c r="I29" s="11">
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
         <v>7.1</v>
       </c>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -2121,8 +2056,8 @@
       <c r="B30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>132</v>
+      <c r="C30" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>3</v>
@@ -2136,19 +2071,19 @@
       <c r="G30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="11">
-        <v>0</v>
-      </c>
-      <c r="I30" s="11">
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
         <v>7.1</v>
       </c>
-      <c r="J30" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K30" s="11">
-        <v>0</v>
-      </c>
-      <c r="L30" s="11">
+      <c r="J30" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K30" s="5">
+        <v>0</v>
+      </c>
+      <c r="L30" s="5">
         <v>7.1</v>
       </c>
     </row>
@@ -2159,7 +2094,7 @@
       <c r="B31" s="2">
         <v>7.1</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -2174,16 +2109,16 @@
       <c r="G31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="5">
         <v>0</v>
       </c>
       <c r="I31" s="2">
         <v>7.2</v>
       </c>
-      <c r="J31" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K31" s="11">
+      <c r="J31" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K31" s="5">
         <v>0</v>
       </c>
       <c r="L31" s="2">
@@ -2197,7 +2132,7 @@
       <c r="B32" s="2">
         <v>7.2</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -2212,14 +2147,14 @@
       <c r="G32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="5">
         <v>0</v>
       </c>
       <c r="I32" s="2">
         <v>7.3</v>
       </c>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2229,7 +2164,7 @@
       <c r="B33" s="2">
         <v>7.3</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -2244,16 +2179,16 @@
       <c r="G33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="5">
         <v>2</v>
       </c>
       <c r="I33" s="2">
         <v>7.4</v>
       </c>
-      <c r="J33" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K33" s="11">
+      <c r="J33" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K33" s="5">
         <v>0</v>
       </c>
       <c r="L33" s="2">
@@ -2267,7 +2202,7 @@
       <c r="B34" s="2">
         <v>7.4</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -2282,16 +2217,16 @@
       <c r="G34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="5">
         <v>0</v>
       </c>
       <c r="I34" s="2">
         <v>8.1</v>
       </c>
-      <c r="J34" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K34" s="11">
+      <c r="J34" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K34" s="5">
         <v>0</v>
       </c>
       <c r="L34" s="2">
@@ -2305,7 +2240,7 @@
       <c r="B35" s="2">
         <v>8.1</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -2320,16 +2255,16 @@
       <c r="G35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="5">
         <v>0</v>
       </c>
       <c r="I35" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="J35" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K35" s="11">
+      <c r="J35" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K35" s="5">
         <v>0</v>
       </c>
       <c r="L35" s="2">
@@ -2343,7 +2278,7 @@
       <c r="B36" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -2358,14 +2293,14 @@
       <c r="G36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H36" s="5">
         <v>0</v>
       </c>
       <c r="I36" s="2">
         <v>8.3000000000000007</v>
       </c>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2375,7 +2310,7 @@
       <c r="B37" s="2">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2390,14 +2325,14 @@
       <c r="G37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H37" s="5">
         <v>0</v>
       </c>
       <c r="I37" s="2">
         <v>8.4</v>
       </c>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2407,7 +2342,7 @@
       <c r="B38" s="2">
         <v>8.4</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2422,16 +2357,16 @@
       <c r="G38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H38" s="5">
         <v>0</v>
       </c>
       <c r="I38" s="2">
         <v>9.1</v>
       </c>
-      <c r="J38" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K38" s="11">
+      <c r="J38" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K38" s="5">
         <v>2</v>
       </c>
       <c r="L38" s="2">
@@ -2445,7 +2380,7 @@
       <c r="B39" s="2">
         <v>9.1</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2460,14 +2395,14 @@
       <c r="G39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="5">
         <v>0</v>
       </c>
       <c r="I39" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
       <c r="L39" s="2"/>
     </row>
     <row r="40" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2477,7 +2412,7 @@
       <c r="B40" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -2492,14 +2427,14 @@
       <c r="G40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H40" s="5">
         <v>0</v>
       </c>
       <c r="I40" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
       <c r="L40" s="2"/>
     </row>
     <row r="41" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2509,7 +2444,7 @@
       <c r="B41" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2524,14 +2459,14 @@
       <c r="G41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="5">
         <v>0</v>
       </c>
       <c r="I41" s="2">
         <v>9.4</v>
       </c>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
       <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2541,7 +2476,7 @@
       <c r="B42" s="2">
         <v>9.4</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2556,14 +2491,14 @@
       <c r="G42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="5">
         <v>0</v>
       </c>
       <c r="I42" s="2">
         <v>10.1</v>
       </c>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2573,7 +2508,7 @@
       <c r="B43" s="2">
         <v>10.1</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -2588,14 +2523,14 @@
       <c r="G43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="5">
         <v>0</v>
       </c>
       <c r="I43" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2605,7 +2540,7 @@
       <c r="B44" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2620,14 +2555,14 @@
       <c r="G44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="5">
         <v>0</v>
       </c>
       <c r="I44" s="2">
         <v>11.1</v>
       </c>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
       <c r="L44" s="2"/>
     </row>
     <row r="45" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2637,7 +2572,7 @@
       <c r="B45" s="2">
         <v>11.1</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2652,14 +2587,14 @@
       <c r="G45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H45" s="5">
         <v>0</v>
       </c>
       <c r="I45" s="2">
         <v>11.2</v>
       </c>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
       <c r="L45" s="2"/>
     </row>
     <row r="46" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2669,7 +2604,7 @@
       <c r="B46" s="2">
         <v>11.2</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -2684,14 +2619,14 @@
       <c r="G46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="5">
         <v>0</v>
       </c>
       <c r="I46" s="2">
         <v>11.3</v>
       </c>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
       <c r="L46" s="2"/>
     </row>
     <row r="47" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2701,7 +2636,7 @@
       <c r="B47" s="2">
         <v>11.3</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -2716,14 +2651,14 @@
       <c r="G47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="5">
         <v>0</v>
       </c>
       <c r="I47" s="2">
         <v>12.1</v>
       </c>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
       <c r="L47" s="2"/>
     </row>
     <row r="48" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2733,7 +2668,7 @@
       <c r="B48" s="2">
         <v>12.1</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="6" t="s">
         <v>61</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -2748,7 +2683,7 @@
       <c r="G48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H48" s="5">
         <v>0</v>
       </c>
       <c r="I48" s="2">
@@ -2762,7 +2697,7 @@
       <c r="B49" s="2">
         <v>12.2</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="6" t="s">
         <v>62</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -2777,7 +2712,7 @@
       <c r="G49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H49" s="5">
         <v>0</v>
       </c>
       <c r="I49" s="2">
@@ -2791,7 +2726,7 @@
       <c r="B50" s="2">
         <v>12.3</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -2806,7 +2741,7 @@
       <c r="G50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H50" s="11">
+      <c r="H50" s="5">
         <v>0</v>
       </c>
       <c r="I50" s="2">
@@ -2820,7 +2755,7 @@
       <c r="B51" s="2">
         <v>12.4</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="6" t="s">
         <v>64</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -2830,20 +2765,20 @@
         <v>2</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H51" s="11">
+      <c r="H51" s="5">
         <v>0</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="13"/>
+      <c r="C86" s="7"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -2857,7 +2792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCB3EEF-6DC6-4B33-BAC3-106D6E5EE2A4}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2868,10 +2803,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2881,334 +2816,159 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0A8E34-6EDA-4FBC-95D6-C915587DA356}">
-  <dimension ref="B1:J32"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="78.85546875" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="6" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="7" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="7" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="7" t="s">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="7" t="s">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="7" t="s">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="7" t="s">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="7" t="s">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="7" t="s">
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="7" t="s">
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="7" t="s">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="7" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="7" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="7" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="7" t="s">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="7" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="7" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="7" t="s">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="7" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="7" t="s">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="7" t="s">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="7" t="s">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="3"/>
     </row>
   </sheetData>
-  <protectedRanges>
-    <protectedRange sqref="B2:B31" name="Range13"/>
-    <protectedRange sqref="C29:C31" name="Range14"/>
-    <protectedRange sqref="D2:D31" name="Range15"/>
-  </protectedRanges>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31" xr:uid="{865A1DEB-9B00-4487-A91C-839FDB73AC72}">
-      <formula1>$H$69:$J$69</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B31" xr:uid="{D73C8682-4955-407A-A716-AFA251D3915D}">
-      <formula1>$H$68:$I$68</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>